<commit_message>
prace nad przjesciami nocnymi jednostek w obiegu
</commit_message>
<xml_diff>
--- a/src/inputs/obiegi/obiegi.xlsx
+++ b/src/inputs/obiegi/obiegi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaspi\Documents\python\nowyObieg\v_1_0_1\src\inputs\obiegi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A830AB84-274C-4151-8E76-5C2BEBC030A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D0B46D-3096-4284-97A3-80D29E050C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>nr_obiegu</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Uwagi</t>
   </si>
   <si>
-    <t>EN57FPS</t>
-  </si>
-  <si>
     <t>815 02</t>
   </si>
   <si>
@@ -57,49 +54,13 @@
     <t>815 03</t>
   </si>
   <si>
-    <t>2x EN57FPS</t>
-  </si>
-  <si>
     <t>EN57ALwKM</t>
   </si>
   <si>
-    <t>815 05</t>
-  </si>
-  <si>
-    <t>815 09</t>
-  </si>
-  <si>
-    <t>815 15</t>
-  </si>
-  <si>
-    <t>815 10</t>
-  </si>
-  <si>
     <t>EN57</t>
   </si>
   <si>
-    <t>815 11</t>
-  </si>
-  <si>
-    <t>815 12</t>
-  </si>
-  <si>
-    <t>815 13</t>
-  </si>
-  <si>
-    <t>815 14</t>
-  </si>
-  <si>
     <t>815 04</t>
-  </si>
-  <si>
-    <t>815 06</t>
-  </si>
-  <si>
-    <t>815 07</t>
-  </si>
-  <si>
-    <t>815 08</t>
   </si>
 </sst>
 </file>
@@ -420,9 +381,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -462,10 +425,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -473,10 +436,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -484,208 +447,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tworzenie szczegolowego dodatku z przebiegu
</commit_message>
<xml_diff>
--- a/src/inputs/obiegi/obiegi.xlsx
+++ b/src/inputs/obiegi/obiegi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaspi\Documents\python\nowyObieg\v_1_0_1\src\inputs\obiegi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D0B46D-3096-4284-97A3-80D29E050C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C824ECB7-D0FA-4376-A494-42524E2845EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>nr_obiegu</t>
   </si>
@@ -45,6 +45,9 @@
     <t>Uwagi</t>
   </si>
   <si>
+    <t>EN57FPS</t>
+  </si>
+  <si>
     <t>815 02</t>
   </si>
   <si>
@@ -54,13 +57,49 @@
     <t>815 03</t>
   </si>
   <si>
+    <t>2x EN57FPS</t>
+  </si>
+  <si>
     <t>EN57ALwKM</t>
   </si>
   <si>
+    <t>815 05</t>
+  </si>
+  <si>
+    <t>815 09</t>
+  </si>
+  <si>
+    <t>815 15</t>
+  </si>
+  <si>
+    <t>815 10</t>
+  </si>
+  <si>
     <t>EN57</t>
   </si>
   <si>
+    <t>815 11</t>
+  </si>
+  <si>
+    <t>815 12</t>
+  </si>
+  <si>
+    <t>815 13</t>
+  </si>
+  <si>
+    <t>815 14</t>
+  </si>
+  <si>
     <t>815 04</t>
+  </si>
+  <si>
+    <t>815 06</t>
+  </si>
+  <si>
+    <t>815 07</t>
+  </si>
+  <si>
+    <t>815 08</t>
   </si>
 </sst>
 </file>
@@ -381,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,10 +464,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -436,10 +475,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -447,10 +486,131 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>